<commit_message>
remove unused function something wrong when parsing data..
</commit_message>
<xml_diff>
--- a/result/201611.xlsx
+++ b/result/201611.xlsx
@@ -3475,7 +3475,7 @@
   <dimension ref="B4:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -3695,6 +3695,12 @@
       <c r="I10">
         <v>9</v>
       </c>
+      <c r="J10">
+        <v>4</v>
+      </c>
+      <c r="K10">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="L10">
         <f t="shared" si="0"/>
         <v>-100</v>
@@ -3765,18 +3771,24 @@
       <c r="B14">
         <v>10</v>
       </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
       <c r="F14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-100</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B15">
         <v>11</v>
       </c>
+      <c r="C15">
+        <v>8</v>
+      </c>
       <c r="F15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-100</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.4">
@@ -3794,7 +3806,7 @@
       </c>
       <c r="F17">
         <f>SUM(F5:F16)</f>
-        <v>510</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
20161126 data update fix simulation bug
</commit_message>
<xml_diff>
--- a/result/201611.xlsx
+++ b/result/201611.xlsx
@@ -2,21 +2,595 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="현재_통합_문서" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="120" windowWidth="11652" windowHeight="6024" activeTab="2"/>
+    <workbookView xWindow="288" yWindow="120" windowWidth="11652" windowHeight="6024" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="13" sheetId="1" r:id="rId1"/>
     <sheet name="19" sheetId="2" r:id="rId2"/>
     <sheet name="20" sheetId="3" r:id="rId3"/>
+    <sheet name="26" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>jyyang</author>
+  </authors>
+  <commentList>
+    <comment ref="D28" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>21,23</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D29" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>124,125,234</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D30" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>1,2,3,4,5</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D33" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2,3</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K33" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>1: 123, 345</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D34" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>21,23</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D35" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>124,125,234</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D36" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>1,2,3,4,5</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D39" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2,3</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K39" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>1: 123, 345</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D40" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>21,23</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K40" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>132,145
+213, 234, 235, 243, 341, 432, 452</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D41" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>124,125,234</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D42" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>143, 153, 154,
+214, 215, 234, 235, 241, 243, 254</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D45" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2,3</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K45" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>1: 123, 345</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D46" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>21,23</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K46" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>132,145
+213, 234, 235, 243, 341, 432, 452</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D47" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>124,125,234</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D48" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>143, 153, 154,
+214, 215, 234, 235, 241, 243, 254, 321, 341, 342, 351, 432, 452</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D51" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2,3</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K51" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>1: 123, 345</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D52" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>21,23</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K52" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>132,145
+213, 234, 235, 243, 341, 432, 452
+531, 541</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D53" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>124,125,234</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D54" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>143, 153, 154,
+214, 215, 234, 235, 241, 243, 254, 321, 341, 342, 351, 432, 452</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D57" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2,3</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D58" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>21,23</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D59" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>124,125,234</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D60" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>143, 
+153, 154,
+214, 215, 
+234, 235, 
+241, 243, 
+254, 321, 
+341, 342, 
+351, 432, 452
+542, 543</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D63" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2,3</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D64" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>21,23</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D65" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>124,125,234</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D66" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>143, 
+153, 154,
+214, 215, 
+234, 235, 
+241, 243, 
+254, 321, 
+341, 342, 
+351, 432, 452
+542, 543</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D69" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2,3</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D70" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>21,23</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D71" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>124,125,234</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D72" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>143, 
+153, 154,
+214, 215, 
+234, 235, 
+241, 243, 
+254, 321, 
+341, 342, 
+351, 432, 452
+542, 543</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="90">
   <si>
     <t xml:space="preserve"> 1st</t>
   </si>
@@ -274,6 +848,38 @@
   </si>
   <si>
     <t>sum</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>복</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>복연</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>쌍</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>삼복</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>삼쌍</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>seoul</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>jeju</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sum:</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -281,7 +887,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -315,6 +921,13 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -338,7 +951,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -348,11 +961,45 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -649,6 +1296,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AF55"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -3114,6 +3762,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="B4:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3472,9 +4121,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="B4:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -3814,4 +4464,1392 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:S73"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q66" sqref="Q66"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="3.5" customWidth="1"/>
+    <col min="2" max="2" width="5.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.59765625" customWidth="1"/>
+    <col min="7" max="7" width="5.09765625" customWidth="1"/>
+    <col min="9" max="9" width="4.19921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.3984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.5" customWidth="1"/>
+    <col min="13" max="13" width="5.09765625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="3.3984375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="2.3984375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.09765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1">
+        <f>SUM(F2:F299)</f>
+        <v>-3501.25</v>
+      </c>
+      <c r="I1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K1" t="s">
+        <v>89</v>
+      </c>
+      <c r="M1">
+        <f>SUM(M2:M300)</f>
+        <v>693.33333333333326</v>
+      </c>
+      <c r="S1">
+        <f>SUM(S2:S300)</f>
+        <v>-200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <f>E3*100-100</f>
+        <v>-100</v>
+      </c>
+      <c r="I3">
+        <v>6</v>
+      </c>
+      <c r="J3">
+        <v>3</v>
+      </c>
+      <c r="K3" t="s">
+        <v>85</v>
+      </c>
+      <c r="L3">
+        <v>15.5</v>
+      </c>
+      <c r="M3">
+        <f>L3*100/6-100</f>
+        <v>158.33333333333331</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <f>E4*100/5-100</f>
+        <v>100</v>
+      </c>
+      <c r="I4">
+        <v>8</v>
+      </c>
+      <c r="J4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>12</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="I6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <f>E9*100-100</f>
+        <v>-100</v>
+      </c>
+      <c r="I9">
+        <v>5</v>
+      </c>
+      <c r="J9">
+        <v>4</v>
+      </c>
+      <c r="K9" t="s">
+        <v>83</v>
+      </c>
+      <c r="L9">
+        <v>6.3</v>
+      </c>
+      <c r="M9">
+        <f>L9*100-100</f>
+        <v>530</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <f>E10*100/2-100</f>
+        <v>-100</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>5</v>
+      </c>
+      <c r="K10" t="s">
+        <v>85</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <f>L10*100/6-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <f t="shared" ref="F11" si="0">E11*100/5-100</f>
+        <v>-100</v>
+      </c>
+      <c r="I11">
+        <v>9</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11" t="s">
+        <v>86</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <f>L11*100/24-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B12">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <f>E12*100/24-100</f>
+        <v>-100</v>
+      </c>
+      <c r="I12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="I13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <f>E15*100-100</f>
+        <v>-100</v>
+      </c>
+      <c r="I15">
+        <v>6</v>
+      </c>
+      <c r="J15">
+        <v>7</v>
+      </c>
+      <c r="K15" t="s">
+        <v>83</v>
+      </c>
+      <c r="L15">
+        <v>1.9</v>
+      </c>
+      <c r="M15">
+        <f>L15*100-100</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B16">
+        <v>12</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <f>E16*100/2-100</f>
+        <v>-100</v>
+      </c>
+      <c r="I16">
+        <v>7</v>
+      </c>
+      <c r="J16">
+        <v>8</v>
+      </c>
+      <c r="K16" t="s">
+        <v>85</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <f>L16*100/6-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="C17">
+        <v>12</v>
+      </c>
+      <c r="D17" t="s">
+        <v>86</v>
+      </c>
+      <c r="E17">
+        <v>38.1</v>
+      </c>
+      <c r="F17">
+        <f>E17*100/24-100</f>
+        <v>58.75</v>
+      </c>
+      <c r="I17">
+        <v>10</v>
+      </c>
+      <c r="J17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B18">
+        <v>8</v>
+      </c>
+      <c r="I18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B19">
+        <v>7</v>
+      </c>
+      <c r="I19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="B21">
+        <v>5</v>
+      </c>
+      <c r="C21">
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <f>E21*100-100</f>
+        <v>-100</v>
+      </c>
+      <c r="I21">
+        <v>6</v>
+      </c>
+      <c r="J21">
+        <v>11</v>
+      </c>
+      <c r="K21" t="s">
+        <v>83</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <f>L21*100-100</f>
+        <v>-100</v>
+      </c>
+      <c r="O21">
+        <v>1</v>
+      </c>
+      <c r="P21">
+        <v>11</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>86</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <f>R21*100/24-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22" t="s">
+        <v>84</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <f>E22*100/2-100</f>
+        <v>-100</v>
+      </c>
+      <c r="I22">
+        <v>2</v>
+      </c>
+      <c r="J22">
+        <v>3</v>
+      </c>
+      <c r="O22">
+        <v>5</v>
+      </c>
+      <c r="P22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B23">
+        <v>8</v>
+      </c>
+      <c r="C23">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s">
+        <v>85</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <f t="shared" ref="F23" si="1">E23*100/5-100</f>
+        <v>-100</v>
+      </c>
+      <c r="I23">
+        <v>7</v>
+      </c>
+      <c r="J23">
+        <v>7</v>
+      </c>
+      <c r="O23">
+        <v>8</v>
+      </c>
+      <c r="P23">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>86</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <f>E24*100/24-100</f>
+        <v>-100</v>
+      </c>
+      <c r="I24">
+        <v>5</v>
+      </c>
+      <c r="O24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B25">
+        <v>9</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A27">
+        <v>5</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>82</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <f>E27*100-100</f>
+        <v>-100</v>
+      </c>
+      <c r="I27">
+        <v>2</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27" t="s">
+        <v>83</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <f>L27*100-100</f>
+        <v>-100</v>
+      </c>
+      <c r="O27">
+        <v>7</v>
+      </c>
+      <c r="P27">
+        <v>1</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>86</v>
+      </c>
+      <c r="R27">
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <f>R27*100/24-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+      <c r="D28" t="s">
+        <v>84</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <f>E28*100/2-100</f>
+        <v>-100</v>
+      </c>
+      <c r="I28">
+        <v>8</v>
+      </c>
+      <c r="J28">
+        <v>3</v>
+      </c>
+      <c r="O28">
+        <v>2</v>
+      </c>
+      <c r="P28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>8</v>
+      </c>
+      <c r="D29" t="s">
+        <v>85</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <f>E29*100/3-100</f>
+        <v>-100</v>
+      </c>
+      <c r="I29">
+        <v>11</v>
+      </c>
+      <c r="J29">
+        <v>7</v>
+      </c>
+      <c r="O29">
+        <v>6</v>
+      </c>
+      <c r="P29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="D30" t="s">
+        <v>86</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <f>E30*100/60-100</f>
+        <v>-100</v>
+      </c>
+      <c r="I30">
+        <v>3</v>
+      </c>
+      <c r="O30">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B31">
+        <v>7</v>
+      </c>
+      <c r="I31">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A33">
+        <v>6</v>
+      </c>
+      <c r="B33">
+        <v>7</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33" t="s">
+        <v>82</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <f>E33*100-100</f>
+        <v>-100</v>
+      </c>
+      <c r="I33">
+        <v>3</v>
+      </c>
+      <c r="J33">
+        <v>10</v>
+      </c>
+      <c r="K33" t="s">
+        <v>85</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+      <c r="M33">
+        <f>L33*100-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>84</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <f>E34*100/2-100</f>
+        <v>-100</v>
+      </c>
+      <c r="I34">
+        <v>1</v>
+      </c>
+      <c r="J34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B35">
+        <v>3</v>
+      </c>
+      <c r="C35">
+        <v>3</v>
+      </c>
+      <c r="D35" t="s">
+        <v>85</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <f>E35*100/3-100</f>
+        <v>-100</v>
+      </c>
+      <c r="I35">
+        <v>8</v>
+      </c>
+      <c r="J35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B36">
+        <v>10</v>
+      </c>
+      <c r="D36" t="s">
+        <v>86</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <f>E36*100/60-100</f>
+        <v>-100</v>
+      </c>
+      <c r="I36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B37">
+        <v>12</v>
+      </c>
+      <c r="C37" s="3"/>
+      <c r="I37">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A39">
+        <v>7</v>
+      </c>
+      <c r="B39">
+        <v>10</v>
+      </c>
+      <c r="C39">
+        <v>9</v>
+      </c>
+      <c r="D39" t="s">
+        <v>82</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <f>E39*100-100</f>
+        <v>-100</v>
+      </c>
+      <c r="I39">
+        <v>9</v>
+      </c>
+      <c r="J39">
+        <v>3</v>
+      </c>
+      <c r="K39" t="s">
+        <v>85</v>
+      </c>
+      <c r="L39">
+        <v>21.5</v>
+      </c>
+      <c r="M39">
+        <f>L39*100/2-100</f>
+        <v>975</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B40">
+        <v>5</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="D40" t="s">
+        <v>84</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <f>E40*100/2-100</f>
+        <v>-100</v>
+      </c>
+      <c r="I40">
+        <v>6</v>
+      </c>
+      <c r="J40">
+        <v>1</v>
+      </c>
+      <c r="K40" t="s">
+        <v>86</v>
+      </c>
+      <c r="L40">
+        <v>0</v>
+      </c>
+      <c r="M40">
+        <f>L40*60/6-60</f>
+        <v>-60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41" t="s">
+        <v>85</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <f>E41*100/3-100</f>
+        <v>-100</v>
+      </c>
+      <c r="I41">
+        <v>3</v>
+      </c>
+      <c r="J41">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B42">
+        <v>4</v>
+      </c>
+      <c r="D42" t="s">
+        <v>86</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <f>E42*100/60-100</f>
+        <v>-100</v>
+      </c>
+      <c r="I42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B43">
+        <v>7</v>
+      </c>
+      <c r="I43">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A45">
+        <v>8</v>
+      </c>
+      <c r="B45">
+        <v>5</v>
+      </c>
+      <c r="C45">
+        <v>6</v>
+      </c>
+      <c r="D45" t="s">
+        <v>82</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <f>E45*100-100</f>
+        <v>-100</v>
+      </c>
+      <c r="I45">
+        <v>2</v>
+      </c>
+      <c r="J45">
+        <v>3</v>
+      </c>
+      <c r="K45" t="s">
+        <v>85</v>
+      </c>
+      <c r="L45">
+        <v>0</v>
+      </c>
+      <c r="M45">
+        <f>L45*100/2-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B46">
+        <v>7</v>
+      </c>
+      <c r="C46">
+        <v>11</v>
+      </c>
+      <c r="D46" t="s">
+        <v>84</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <f>E46*100/2-100</f>
+        <v>-100</v>
+      </c>
+      <c r="I46">
+        <v>1</v>
+      </c>
+      <c r="J46">
+        <v>2</v>
+      </c>
+      <c r="K46" t="s">
+        <v>86</v>
+      </c>
+      <c r="L46">
+        <v>0</v>
+      </c>
+      <c r="M46">
+        <f>L46*100/9-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B47">
+        <v>8</v>
+      </c>
+      <c r="C47">
+        <v>7</v>
+      </c>
+      <c r="D47" t="s">
+        <v>85</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <f>E47*100/3-100</f>
+        <v>-100</v>
+      </c>
+      <c r="I47">
+        <v>3</v>
+      </c>
+      <c r="J47">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B48">
+        <v>3</v>
+      </c>
+      <c r="D48" t="s">
+        <v>86</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <f>E48*100/16-100</f>
+        <v>-100</v>
+      </c>
+      <c r="I48">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B49">
+        <v>12</v>
+      </c>
+      <c r="I49">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A51">
+        <v>9</v>
+      </c>
+      <c r="B51">
+        <v>6</v>
+      </c>
+      <c r="C51">
+        <v>12</v>
+      </c>
+      <c r="D51" t="s">
+        <v>82</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <f>E51*100-100</f>
+        <v>-100</v>
+      </c>
+      <c r="I51">
+        <v>4</v>
+      </c>
+      <c r="J51">
+        <v>6</v>
+      </c>
+      <c r="K51" t="s">
+        <v>85</v>
+      </c>
+      <c r="L51">
+        <v>0</v>
+      </c>
+      <c r="M51">
+        <f>L51*100/2-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B52">
+        <v>3</v>
+      </c>
+      <c r="C52">
+        <v>3</v>
+      </c>
+      <c r="D52" t="s">
+        <v>84</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52">
+        <f>E52*100/2-100</f>
+        <v>-100</v>
+      </c>
+      <c r="I52">
+        <v>2</v>
+      </c>
+      <c r="J52">
+        <v>5</v>
+      </c>
+      <c r="K52" t="s">
+        <v>86</v>
+      </c>
+      <c r="L52">
+        <v>0</v>
+      </c>
+      <c r="M52">
+        <f>L52*100/11-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B53">
+        <v>11</v>
+      </c>
+      <c r="C53">
+        <v>4</v>
+      </c>
+      <c r="D53" t="s">
+        <v>85</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <f>E53*100/3-100</f>
+        <v>-100</v>
+      </c>
+      <c r="I53">
+        <v>6</v>
+      </c>
+      <c r="J53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B54">
+        <v>5</v>
+      </c>
+      <c r="D54" t="s">
+        <v>86</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <f>E54*100/16-100</f>
+        <v>-100</v>
+      </c>
+      <c r="I54">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B55">
+        <v>12</v>
+      </c>
+      <c r="I55">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A57">
+        <v>10</v>
+      </c>
+      <c r="B57">
+        <v>10</v>
+      </c>
+      <c r="C57">
+        <v>8</v>
+      </c>
+      <c r="D57" t="s">
+        <v>82</v>
+      </c>
+      <c r="E57">
+        <v>6.4</v>
+      </c>
+      <c r="F57">
+        <f>E57*100-100</f>
+        <v>540</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B58">
+        <v>5</v>
+      </c>
+      <c r="C58">
+        <v>5</v>
+      </c>
+      <c r="D58" t="s">
+        <v>84</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <f>E58*100/2-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B59">
+        <v>8</v>
+      </c>
+      <c r="C59">
+        <v>4</v>
+      </c>
+      <c r="D59" t="s">
+        <v>85</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <f>E59*100/3-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B60">
+        <v>6</v>
+      </c>
+      <c r="D60" t="s">
+        <v>86</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <f>E60*100/16-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B61">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A63">
+        <v>11</v>
+      </c>
+      <c r="B63">
+        <v>12</v>
+      </c>
+      <c r="D63" t="s">
+        <v>82</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <f>E63*100-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B64">
+        <v>11</v>
+      </c>
+      <c r="D64" t="s">
+        <v>84</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <f>E64*100/2-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B65">
+        <v>7</v>
+      </c>
+      <c r="D65" t="s">
+        <v>85</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <f>E65*100/3-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B66">
+        <v>4</v>
+      </c>
+      <c r="D66" t="s">
+        <v>86</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66">
+        <f>E66*100/16-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B67">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A69">
+        <v>12</v>
+      </c>
+      <c r="B69">
+        <v>3</v>
+      </c>
+      <c r="D69" t="s">
+        <v>82</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <f>E69*100-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B70">
+        <v>7</v>
+      </c>
+      <c r="D70" t="s">
+        <v>84</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <f>E70*100/2-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B71">
+        <v>8</v>
+      </c>
+      <c r="D71" t="s">
+        <v>85</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <f>E71*100/3-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B72">
+        <v>2</v>
+      </c>
+      <c r="D72" t="s">
+        <v>86</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <f>E72*100/16-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B73">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="G40:G49">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>G40&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H49">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>H49&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H45:H48">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>H45&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N45:N47">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>N45&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add function to get race record update 20161127 race
</commit_message>
<xml_diff>
--- a/result/201611.xlsx
+++ b/result/201611.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="현재_통합_문서" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="120" windowWidth="11652" windowHeight="6024" activeTab="3"/>
+    <workbookView xWindow="288" yWindow="120" windowWidth="11652" windowHeight="6024" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="13" sheetId="1" r:id="rId1"/>
     <sheet name="19" sheetId="2" r:id="rId2"/>
     <sheet name="20" sheetId="3" r:id="rId3"/>
     <sheet name="26" sheetId="4" r:id="rId4"/>
+    <sheet name="27" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -589,8 +590,40 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>jyyang</author>
+  </authors>
+  <commentList>
+    <comment ref="D35" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>143, 
+153, 154,
+214, 215, 
+234, 235, 
+241, 243, 
+254, 321, 
+341, 342, 
+351, 432, 452
+542, 543</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="98">
   <si>
     <t xml:space="preserve"> 1st</t>
   </si>
@@ -880,6 +913,38 @@
   </si>
   <si>
     <t>sum:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>busan</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>b</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>s</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sb</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ss</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>d</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>by</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ss</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -968,13 +1033,7 @@
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <b/>
@@ -4471,9 +4530,9 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:S73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q66" sqref="Q66"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -5698,6 +5757,9 @@
       <c r="B63">
         <v>12</v>
       </c>
+      <c r="C63">
+        <v>6</v>
+      </c>
       <c r="D63" t="s">
         <v>82</v>
       </c>
@@ -5713,6 +5775,9 @@
       <c r="B64">
         <v>11</v>
       </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
       <c r="D64" t="s">
         <v>84</v>
       </c>
@@ -5727,6 +5792,9 @@
     <row r="65" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B65">
         <v>7</v>
+      </c>
+      <c r="C65">
+        <v>4</v>
       </c>
       <c r="D65" t="s">
         <v>85</v>
@@ -5766,6 +5834,9 @@
       <c r="B69">
         <v>3</v>
       </c>
+      <c r="C69">
+        <v>6</v>
+      </c>
       <c r="D69" t="s">
         <v>82</v>
       </c>
@@ -5780,6 +5851,9 @@
     <row r="70" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B70">
         <v>7</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
       </c>
       <c r="D70" t="s">
         <v>84</v>
@@ -5795,6 +5869,9 @@
     <row r="71" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B71">
         <v>8</v>
+      </c>
+      <c r="C71">
+        <v>9</v>
       </c>
       <c r="D71" t="s">
         <v>85</v>
@@ -5852,4 +5929,1060 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M66"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G61" sqref="G61"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="3.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.5" customWidth="1"/>
+    <col min="4" max="4" width="5.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.59765625" customWidth="1"/>
+    <col min="8" max="8" width="2.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.19921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4" customWidth="1"/>
+    <col min="11" max="11" width="5.19921875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.3984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.09765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1">
+        <f>SUM(F2:F299)</f>
+        <v>-1116.1666666666667</v>
+      </c>
+      <c r="I1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K1" t="s">
+        <v>89</v>
+      </c>
+      <c r="M1">
+        <f>SUM(M15:M300)</f>
+        <v>4316.6666666666661</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f>E2*100-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B3">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <f>E3*100/2-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B4">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <f>E4*100/3-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <f>E5*100/18-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <f>E8*100-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>92</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <f>E9*100/2-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B10">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>93</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <f>E10*100/3-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B11">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <f>E11*100/18-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <f>E14*100-100</f>
+        <v>-100</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>6</v>
+      </c>
+      <c r="J14">
+        <v>9</v>
+      </c>
+      <c r="K14" t="s">
+        <v>95</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <f>L14*100-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s">
+        <v>92</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <f>E15*100/2-100</f>
+        <v>-100</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>5</v>
+      </c>
+      <c r="K15" t="s">
+        <v>91</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <f>L15*100-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
+        <v>93</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <f>E16*100/3-100</f>
+        <v>-100</v>
+      </c>
+      <c r="I16">
+        <v>8</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16" t="s">
+        <v>96</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <f>L16*100-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <f>E17*100/18-100</f>
+        <v>-100</v>
+      </c>
+      <c r="I17">
+        <v>7</v>
+      </c>
+      <c r="K17" t="s">
+        <v>92</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <f>L17*100/2-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B18">
+        <v>10</v>
+      </c>
+      <c r="I18">
+        <v>4</v>
+      </c>
+      <c r="K18" t="s">
+        <v>93</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <f>L18*100/3-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="K19" t="s">
+        <v>94</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <f>L19*100/16-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A20">
+        <v>4</v>
+      </c>
+      <c r="B20">
+        <v>7</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>91</v>
+      </c>
+      <c r="E20">
+        <v>7.8</v>
+      </c>
+      <c r="F20">
+        <f>E20*100-100</f>
+        <v>680</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B21">
+        <v>12</v>
+      </c>
+      <c r="C21">
+        <v>12</v>
+      </c>
+      <c r="D21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <f>E21*100/2-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>5</v>
+      </c>
+      <c r="D22" t="s">
+        <v>93</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <f>E22*100/3-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>94</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <f>E23*100/18-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B24">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A26">
+        <v>5</v>
+      </c>
+      <c r="B26">
+        <v>8</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>91</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <f>E26*100-100</f>
+        <v>-100</v>
+      </c>
+      <c r="H26">
+        <v>2</v>
+      </c>
+      <c r="I26">
+        <v>10</v>
+      </c>
+      <c r="J26">
+        <v>7</v>
+      </c>
+      <c r="K26" t="s">
+        <v>95</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <f>L26*100-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B27">
+        <v>12</v>
+      </c>
+      <c r="C27">
+        <v>8</v>
+      </c>
+      <c r="D27" t="s">
+        <v>92</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <f>E27*100/2-100</f>
+        <v>-100</v>
+      </c>
+      <c r="I27">
+        <v>2</v>
+      </c>
+      <c r="J27">
+        <v>6</v>
+      </c>
+      <c r="K27" t="s">
+        <v>91</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <f>L27*100-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28">
+        <v>6</v>
+      </c>
+      <c r="D28" t="s">
+        <v>93</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <f>E28*100/3-100</f>
+        <v>-100</v>
+      </c>
+      <c r="I28">
+        <v>8</v>
+      </c>
+      <c r="K28" t="s">
+        <v>96</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <f>L28*100-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B29">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
+        <v>94</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <f>E29*100/18-100</f>
+        <v>-100</v>
+      </c>
+      <c r="I29">
+        <v>4</v>
+      </c>
+      <c r="K29" t="s">
+        <v>92</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <f>L29*100/2-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B30">
+        <v>7</v>
+      </c>
+      <c r="I30">
+        <v>3</v>
+      </c>
+      <c r="K30" t="s">
+        <v>93</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <f>L30*100/3-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="K31" t="s">
+        <v>94</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <f>L31*100/16-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A32">
+        <v>6</v>
+      </c>
+      <c r="B32">
+        <v>8</v>
+      </c>
+      <c r="C32">
+        <v>11</v>
+      </c>
+      <c r="D32" t="s">
+        <v>91</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <f>E32*100-100</f>
+        <v>-100</v>
+      </c>
+      <c r="H32">
+        <v>3</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="J32">
+        <v>8</v>
+      </c>
+      <c r="K32" t="s">
+        <v>91</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <f>L32*100-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B33">
+        <v>10</v>
+      </c>
+      <c r="C33">
+        <v>8</v>
+      </c>
+      <c r="D33" t="s">
+        <v>92</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <f>E33*100/2-100</f>
+        <v>-100</v>
+      </c>
+      <c r="I33">
+        <v>5</v>
+      </c>
+      <c r="J33">
+        <v>12</v>
+      </c>
+      <c r="K33" t="s">
+        <v>96</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+      <c r="M33">
+        <f>L33*100-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B34">
+        <v>11</v>
+      </c>
+      <c r="C34">
+        <v>9</v>
+      </c>
+      <c r="D34" t="s">
+        <v>93</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <f>E34*100/3-100</f>
+        <v>-100</v>
+      </c>
+      <c r="I34">
+        <v>9</v>
+      </c>
+      <c r="J34">
+        <v>11</v>
+      </c>
+      <c r="K34" t="s">
+        <v>93</v>
+      </c>
+      <c r="L34">
+        <v>0</v>
+      </c>
+      <c r="M34">
+        <f>L34*100-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="D35" t="s">
+        <v>97</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <f>E35*100/18-100</f>
+        <v>-100</v>
+      </c>
+      <c r="I35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B36">
+        <v>9</v>
+      </c>
+      <c r="I36">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A38">
+        <v>7</v>
+      </c>
+      <c r="B38">
+        <v>7</v>
+      </c>
+      <c r="C38">
+        <v>11</v>
+      </c>
+      <c r="D38" t="s">
+        <v>94</v>
+      </c>
+      <c r="E38">
+        <v>225.3</v>
+      </c>
+      <c r="F38">
+        <f>E38*100/60-100</f>
+        <v>275.5</v>
+      </c>
+      <c r="H38">
+        <v>4</v>
+      </c>
+      <c r="I38">
+        <v>9</v>
+      </c>
+      <c r="J38">
+        <v>5</v>
+      </c>
+      <c r="K38" t="s">
+        <v>94</v>
+      </c>
+      <c r="L38">
+        <v>3443</v>
+      </c>
+      <c r="M38">
+        <f>L38*100/60-100</f>
+        <v>5638.333333333333</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>4</v>
+      </c>
+      <c r="I39">
+        <v>11</v>
+      </c>
+      <c r="J39">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B40">
+        <v>11</v>
+      </c>
+      <c r="C40">
+        <v>7</v>
+      </c>
+      <c r="I40">
+        <v>5</v>
+      </c>
+      <c r="J40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B41">
+        <v>6</v>
+      </c>
+      <c r="I41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B42">
+        <v>4</v>
+      </c>
+      <c r="I42">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A44">
+        <v>8</v>
+      </c>
+      <c r="B44">
+        <v>10</v>
+      </c>
+      <c r="C44">
+        <v>10</v>
+      </c>
+      <c r="D44" t="s">
+        <v>94</v>
+      </c>
+      <c r="E44">
+        <v>257</v>
+      </c>
+      <c r="F44">
+        <f>E44*100/60-100</f>
+        <v>328.33333333333331</v>
+      </c>
+      <c r="H44">
+        <v>5</v>
+      </c>
+      <c r="I44">
+        <v>5</v>
+      </c>
+      <c r="J44">
+        <v>12</v>
+      </c>
+      <c r="K44" t="s">
+        <v>94</v>
+      </c>
+      <c r="L44">
+        <v>0</v>
+      </c>
+      <c r="M44">
+        <f>L44*100/60-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B45">
+        <v>8</v>
+      </c>
+      <c r="C45">
+        <v>6</v>
+      </c>
+      <c r="I45">
+        <v>11</v>
+      </c>
+      <c r="J45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B46">
+        <v>3</v>
+      </c>
+      <c r="C46">
+        <v>3</v>
+      </c>
+      <c r="I46">
+        <v>2</v>
+      </c>
+      <c r="J46">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B47">
+        <v>7</v>
+      </c>
+      <c r="I47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B48">
+        <v>6</v>
+      </c>
+      <c r="I48">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A50">
+        <v>9</v>
+      </c>
+      <c r="B50">
+        <v>4</v>
+      </c>
+      <c r="C50">
+        <v>11</v>
+      </c>
+      <c r="D50" t="s">
+        <v>94</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <f>E50*100/60-100</f>
+        <v>-100</v>
+      </c>
+      <c r="H50">
+        <v>6</v>
+      </c>
+      <c r="I50">
+        <v>4</v>
+      </c>
+      <c r="J50">
+        <v>7</v>
+      </c>
+      <c r="K50" t="s">
+        <v>94</v>
+      </c>
+      <c r="L50">
+        <v>167</v>
+      </c>
+      <c r="M50">
+        <f>L50*100/60-100</f>
+        <v>178.33333333333331</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B51">
+        <v>5</v>
+      </c>
+      <c r="C51">
+        <v>9</v>
+      </c>
+      <c r="I51">
+        <v>7</v>
+      </c>
+      <c r="J51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B52">
+        <v>3</v>
+      </c>
+      <c r="C52">
+        <v>4</v>
+      </c>
+      <c r="I52">
+        <v>5</v>
+      </c>
+      <c r="J52">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B53">
+        <v>2</v>
+      </c>
+      <c r="I53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B54">
+        <v>12</v>
+      </c>
+      <c r="I54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A56">
+        <v>10</v>
+      </c>
+      <c r="B56">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B57">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B58">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B59">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A62">
+        <v>11</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B63">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B64">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B65">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B66">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
nan data fill with median value
</commit_message>
<xml_diff>
--- a/result/201611.xlsx
+++ b/result/201611.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="현재_통합_문서" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\study\kra\result\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="288" yWindow="120" windowWidth="11652" windowHeight="6024" activeTab="4"/>
+    <workbookView xWindow="2070" yWindow="120" windowWidth="11655" windowHeight="6030" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="13" sheetId="1" r:id="rId1"/>
@@ -13,7 +18,7 @@
     <sheet name="26" sheetId="4" r:id="rId4"/>
     <sheet name="27" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -23,7 +28,7 @@
     <author>jyyang</author>
   </authors>
   <commentList>
-    <comment ref="D28" authorId="0">
+    <comment ref="D28" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -37,7 +42,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D29" authorId="0">
+    <comment ref="D29" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -51,7 +56,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D30" authorId="0">
+    <comment ref="D30" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -65,7 +70,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D33" authorId="0">
+    <comment ref="D33" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -79,7 +84,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K33" authorId="0">
+    <comment ref="K33" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -93,7 +98,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D34" authorId="0">
+    <comment ref="D34" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -107,7 +112,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D35" authorId="0">
+    <comment ref="D35" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -121,7 +126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D36" authorId="0">
+    <comment ref="D36" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -135,7 +140,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D39" authorId="0">
+    <comment ref="D39" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -149,7 +154,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K39" authorId="0">
+    <comment ref="K39" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -163,7 +168,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D40" authorId="0">
+    <comment ref="D40" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -177,7 +182,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K40" authorId="0">
+    <comment ref="K40" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -192,7 +197,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D41" authorId="0">
+    <comment ref="D41" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -206,7 +211,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D42" authorId="0">
+    <comment ref="D42" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -221,7 +226,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D45" authorId="0">
+    <comment ref="D45" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -235,7 +240,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K45" authorId="0">
+    <comment ref="K45" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -249,7 +254,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D46" authorId="0">
+    <comment ref="D46" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -263,7 +268,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K46" authorId="0">
+    <comment ref="K46" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -278,7 +283,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D47" authorId="0">
+    <comment ref="D47" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -292,7 +297,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D48" authorId="0">
+    <comment ref="D48" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -307,7 +312,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D51" authorId="0">
+    <comment ref="D51" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -321,7 +326,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K51" authorId="0">
+    <comment ref="K51" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -335,7 +340,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D52" authorId="0">
+    <comment ref="D52" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -349,7 +354,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K52" authorId="0">
+    <comment ref="K52" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -365,7 +370,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D53" authorId="0">
+    <comment ref="D53" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -379,7 +384,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D54" authorId="0">
+    <comment ref="D54" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -394,7 +399,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D57" authorId="0">
+    <comment ref="D57" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -408,7 +413,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D58" authorId="0">
+    <comment ref="D58" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -422,7 +427,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D59" authorId="0">
+    <comment ref="D59" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -436,7 +441,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D60" authorId="0">
+    <comment ref="D60" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -458,7 +463,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D63" authorId="0">
+    <comment ref="D63" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -472,7 +477,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D64" authorId="0">
+    <comment ref="D64" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -486,7 +491,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D65" authorId="0">
+    <comment ref="D65" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -500,7 +505,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D66" authorId="0">
+    <comment ref="D66" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -522,7 +527,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D69" authorId="0">
+    <comment ref="D69" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -536,7 +541,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D70" authorId="0">
+    <comment ref="D70" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -550,7 +555,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D71" authorId="0">
+    <comment ref="D71" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -564,7 +569,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D72" authorId="0">
+    <comment ref="D72" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -596,7 +601,7 @@
     <author>jyyang</author>
   </authors>
   <commentList>
-    <comment ref="D35" authorId="0">
+    <comment ref="D35" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -623,7 +628,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="99">
   <si>
     <t xml:space="preserve"> 1st</t>
   </si>
@@ -941,6 +946,10 @@
   </si>
   <si>
     <t>by</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ss</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -1064,6 +1073,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1111,7 +1123,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1146,7 +1158,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1363,41 +1375,41 @@
       <selection pane="bottomLeft" activeCell="AE51" sqref="AE51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.09765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.59765625" customWidth="1"/>
-    <col min="4" max="4" width="6.09765625" customWidth="1"/>
-    <col min="5" max="5" width="4.3984375" customWidth="1"/>
+    <col min="1" max="1" width="3.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.625" customWidth="1"/>
+    <col min="4" max="4" width="6.125" customWidth="1"/>
+    <col min="5" max="5" width="4.375" customWidth="1"/>
     <col min="6" max="6" width="3" customWidth="1"/>
-    <col min="7" max="7" width="5.09765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6" customWidth="1"/>
-    <col min="10" max="10" width="3.09765625" customWidth="1"/>
+    <col min="10" max="10" width="3.125" customWidth="1"/>
     <col min="11" max="11" width="3.5" customWidth="1"/>
-    <col min="12" max="12" width="5.09765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="6" customWidth="1"/>
     <col min="15" max="15" width="3.5" customWidth="1"/>
-    <col min="16" max="16" width="3.69921875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3.75" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="6.5" customWidth="1"/>
-    <col min="18" max="18" width="13.59765625" customWidth="1"/>
-    <col min="19" max="19" width="6.296875" customWidth="1"/>
-    <col min="20" max="20" width="3.69921875" customWidth="1"/>
-    <col min="21" max="21" width="3.296875" customWidth="1"/>
-    <col min="22" max="22" width="5.09765625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.8984375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.296875" customWidth="1"/>
-    <col min="25" max="25" width="3.3984375" customWidth="1"/>
+    <col min="18" max="18" width="13.625" customWidth="1"/>
+    <col min="19" max="19" width="6.25" customWidth="1"/>
+    <col min="20" max="20" width="3.75" customWidth="1"/>
+    <col min="21" max="21" width="3.25" customWidth="1"/>
+    <col min="22" max="22" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.25" customWidth="1"/>
+    <col min="25" max="25" width="3.375" customWidth="1"/>
     <col min="26" max="26" width="3.5" customWidth="1"/>
-    <col min="27" max="27" width="5.09765625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.8984375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="6.296875" customWidth="1"/>
-    <col min="30" max="30" width="4.3984375" customWidth="1"/>
+    <col min="27" max="27" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="6.25" customWidth="1"/>
+    <col min="30" max="30" width="4.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -1420,7 +1432,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1476,7 +1488,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -1537,7 +1549,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1590,7 +1602,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1646,7 +1658,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1699,7 +1711,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>2</v>
       </c>
@@ -1760,7 +1772,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>3</v>
       </c>
@@ -1828,7 +1840,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>3</v>
       </c>
@@ -1893,7 +1905,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>3</v>
       </c>
@@ -1958,7 +1970,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>4</v>
       </c>
@@ -2038,7 +2050,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>4</v>
       </c>
@@ -2115,7 +2127,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>4</v>
       </c>
@@ -2192,7 +2204,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>5</v>
       </c>
@@ -2272,7 +2284,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>5</v>
       </c>
@@ -2349,7 +2361,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>5</v>
       </c>
@@ -2426,7 +2438,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>6</v>
       </c>
@@ -2506,7 +2518,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>6</v>
       </c>
@@ -2583,7 +2595,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>6</v>
       </c>
@@ -2660,7 +2672,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>7</v>
       </c>
@@ -2740,7 +2752,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="34" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>7</v>
       </c>
@@ -2817,7 +2829,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>7</v>
       </c>
@@ -2894,7 +2906,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>8</v>
       </c>
@@ -2974,7 +2986,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="39" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>8</v>
       </c>
@@ -3051,7 +3063,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>8</v>
       </c>
@@ -3128,7 +3140,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>9</v>
       </c>
@@ -3205,7 +3217,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>9</v>
       </c>
@@ -3282,7 +3294,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>9</v>
       </c>
@@ -3359,7 +3371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>10</v>
       </c>
@@ -3436,7 +3448,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>10</v>
       </c>
@@ -3513,7 +3525,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>10</v>
       </c>
@@ -3590,7 +3602,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>11</v>
       </c>
@@ -3664,7 +3676,7 @@
         <v>872.17</v>
       </c>
     </row>
-    <row r="54" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>11</v>
       </c>
@@ -3738,7 +3750,7 @@
         <v>871.3</v>
       </c>
     </row>
-    <row r="55" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>11</v>
       </c>
@@ -3828,21 +3840,21 @@
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="4.796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.09765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.09765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.3984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.09765625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.3984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.09765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.75" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>78</v>
       </c>
@@ -3862,7 +3874,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>1</v>
       </c>
@@ -3887,7 +3899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>2</v>
       </c>
@@ -3912,7 +3924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>3</v>
       </c>
@@ -3937,7 +3949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>4</v>
       </c>
@@ -3971,7 +3983,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>5</v>
       </c>
@@ -4005,7 +4017,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>6</v>
       </c>
@@ -4030,7 +4042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>7</v>
       </c>
@@ -4055,7 +4067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>8</v>
       </c>
@@ -4080,7 +4092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>9</v>
       </c>
@@ -4105,7 +4117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>10</v>
       </c>
@@ -4123,7 +4135,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>11</v>
       </c>
@@ -4141,7 +4153,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>12</v>
       </c>
@@ -4159,7 +4171,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>81</v>
       </c>
@@ -4187,20 +4199,20 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="4.796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="3.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.09765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.09765625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="3.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.75" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.09765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="I4" t="s">
         <v>78</v>
       </c>
@@ -4211,7 +4223,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>1</v>
       </c>
@@ -4245,7 +4257,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>2</v>
       </c>
@@ -4279,7 +4291,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>3</v>
       </c>
@@ -4313,7 +4325,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>4</v>
       </c>
@@ -4347,7 +4359,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>5</v>
       </c>
@@ -4381,7 +4393,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>6</v>
       </c>
@@ -4415,7 +4427,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>7</v>
       </c>
@@ -4440,7 +4452,7 @@
         <v>-160</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>8</v>
       </c>
@@ -4458,7 +4470,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>9</v>
       </c>
@@ -4476,7 +4488,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>10</v>
       </c>
@@ -4488,7 +4500,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>11</v>
       </c>
@@ -4500,7 +4512,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>12</v>
       </c>
@@ -4509,7 +4521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>81</v>
       </c>
@@ -4535,27 +4547,27 @@
       <selection pane="bottomLeft" activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.5" customWidth="1"/>
-    <col min="2" max="2" width="5.69921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.59765625" customWidth="1"/>
-    <col min="7" max="7" width="5.09765625" customWidth="1"/>
-    <col min="9" max="9" width="4.19921875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.625" customWidth="1"/>
+    <col min="7" max="7" width="5.125" customWidth="1"/>
+    <col min="9" max="9" width="4.25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5.5" customWidth="1"/>
-    <col min="13" max="13" width="5.09765625" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="3.3984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="3.375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="2.3984375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.09765625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="2.375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>87</v>
       </c>
@@ -4581,7 +4593,7 @@
         <v>-200</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4618,7 +4630,7 @@
         <v>158.33333333333331</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>2</v>
       </c>
@@ -4642,7 +4654,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>3</v>
       </c>
@@ -4656,7 +4668,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>8</v>
       </c>
@@ -4664,7 +4676,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>6</v>
       </c>
@@ -4672,7 +4684,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2</v>
       </c>
@@ -4709,7 +4721,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>1</v>
       </c>
@@ -4743,7 +4755,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>5</v>
       </c>
@@ -4777,7 +4789,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>7</v>
       </c>
@@ -4795,7 +4807,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>10</v>
       </c>
@@ -4803,7 +4815,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>3</v>
       </c>
@@ -4840,7 +4852,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>12</v>
       </c>
@@ -4874,7 +4886,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>10</v>
       </c>
@@ -4898,7 +4910,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>8</v>
       </c>
@@ -4906,7 +4918,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>7</v>
       </c>
@@ -4914,7 +4926,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>4</v>
       </c>
@@ -4967,7 +4979,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>3</v>
       </c>
@@ -4997,7 +5009,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>8</v>
       </c>
@@ -5027,7 +5039,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>2</v>
       </c>
@@ -5048,7 +5060,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>9</v>
       </c>
@@ -5056,7 +5068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>5</v>
       </c>
@@ -5109,7 +5121,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>5</v>
       </c>
@@ -5139,7 +5151,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>3</v>
       </c>
@@ -5169,7 +5181,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>4</v>
       </c>
@@ -5190,7 +5202,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B31">
         <v>7</v>
       </c>
@@ -5198,7 +5210,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>6</v>
       </c>
@@ -5235,7 +5247,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B34">
         <v>2</v>
       </c>
@@ -5259,7 +5271,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B35">
         <v>3</v>
       </c>
@@ -5283,7 +5295,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B36">
         <v>10</v>
       </c>
@@ -5301,7 +5313,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B37">
         <v>12</v>
       </c>
@@ -5310,7 +5322,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>7</v>
       </c>
@@ -5347,7 +5359,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B40">
         <v>5</v>
       </c>
@@ -5381,7 +5393,7 @@
         <v>-60</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B41">
         <v>2</v>
       </c>
@@ -5405,7 +5417,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B42">
         <v>4</v>
       </c>
@@ -5423,7 +5435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B43">
         <v>7</v>
       </c>
@@ -5431,7 +5443,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>8</v>
       </c>
@@ -5468,7 +5480,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B46">
         <v>7</v>
       </c>
@@ -5502,7 +5514,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B47">
         <v>8</v>
       </c>
@@ -5526,7 +5538,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B48">
         <v>3</v>
       </c>
@@ -5544,7 +5556,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B49">
         <v>12</v>
       </c>
@@ -5552,7 +5564,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>9</v>
       </c>
@@ -5589,7 +5601,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B52">
         <v>3</v>
       </c>
@@ -5623,7 +5635,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B53">
         <v>11</v>
       </c>
@@ -5647,7 +5659,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B54">
         <v>5</v>
       </c>
@@ -5665,7 +5677,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B55">
         <v>12</v>
       </c>
@@ -5673,7 +5685,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>10</v>
       </c>
@@ -5694,7 +5706,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B58">
         <v>5</v>
       </c>
@@ -5712,7 +5724,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B59">
         <v>8</v>
       </c>
@@ -5730,7 +5742,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B60">
         <v>6</v>
       </c>
@@ -5745,12 +5757,12 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B61">
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>11</v>
       </c>
@@ -5771,7 +5783,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B64">
         <v>11</v>
       </c>
@@ -5789,7 +5801,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B65">
         <v>7</v>
       </c>
@@ -5807,7 +5819,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B66">
         <v>4</v>
       </c>
@@ -5822,12 +5834,12 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B67">
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>12</v>
       </c>
@@ -5848,7 +5860,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B70">
         <v>7</v>
       </c>
@@ -5866,7 +5878,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B71">
         <v>8</v>
       </c>
@@ -5884,7 +5896,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B72">
         <v>2</v>
       </c>
@@ -5899,7 +5911,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B73">
         <v>9</v>
       </c>
@@ -5937,26 +5949,26 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G61" sqref="G61"/>
+      <selection pane="bottomLeft" activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.69921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.75" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.5" customWidth="1"/>
-    <col min="4" max="4" width="5.19921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.59765625" customWidth="1"/>
-    <col min="8" max="8" width="2.3984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.625" customWidth="1"/>
+    <col min="8" max="8" width="2.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.25" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4" customWidth="1"/>
-    <col min="11" max="11" width="5.19921875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.3984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.09765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>87</v>
       </c>
@@ -5965,7 +5977,7 @@
       </c>
       <c r="F1">
         <f>SUM(F2:F299)</f>
-        <v>-1116.1666666666667</v>
+        <v>5065.5</v>
       </c>
       <c r="I1" t="s">
         <v>90</v>
@@ -5978,7 +5990,7 @@
         <v>4316.6666666666661</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5999,7 +6011,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>7</v>
       </c>
@@ -6017,7 +6029,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>9</v>
       </c>
@@ -6035,7 +6047,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>4</v>
       </c>
@@ -6050,12 +6062,12 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2</v>
       </c>
@@ -6076,7 +6088,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>1</v>
       </c>
@@ -6094,7 +6106,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>11</v>
       </c>
@@ -6112,7 +6124,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>6</v>
       </c>
@@ -6127,12 +6139,12 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>3</v>
       </c>
@@ -6172,7 +6184,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>2</v>
       </c>
@@ -6206,7 +6218,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>3</v>
       </c>
@@ -6240,7 +6252,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>5</v>
       </c>
@@ -6268,7 +6280,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>10</v>
       </c>
@@ -6286,7 +6298,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="K19" t="s">
         <v>94</v>
       </c>
@@ -6298,7 +6310,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>4</v>
       </c>
@@ -6319,7 +6331,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>12</v>
       </c>
@@ -6337,7 +6349,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>2</v>
       </c>
@@ -6355,7 +6367,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>1</v>
       </c>
@@ -6370,12 +6382,12 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>5</v>
       </c>
@@ -6415,7 +6427,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>12</v>
       </c>
@@ -6449,7 +6461,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>5</v>
       </c>
@@ -6480,7 +6492,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>6</v>
       </c>
@@ -6508,7 +6520,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>7</v>
       </c>
@@ -6526,7 +6538,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="K31" t="s">
         <v>94</v>
       </c>
@@ -6538,7 +6550,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>6</v>
       </c>
@@ -6578,7 +6590,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B33">
         <v>10</v>
       </c>
@@ -6612,7 +6624,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B34">
         <v>11</v>
       </c>
@@ -6646,7 +6658,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B35">
         <v>1</v>
       </c>
@@ -6664,7 +6676,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B36">
         <v>9</v>
       </c>
@@ -6672,7 +6684,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>7</v>
       </c>
@@ -6712,7 +6724,7 @@
         <v>5638.333333333333</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B39">
         <v>1</v>
       </c>
@@ -6726,7 +6738,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B40">
         <v>11</v>
       </c>
@@ -6740,7 +6752,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B41">
         <v>6</v>
       </c>
@@ -6748,7 +6760,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B42">
         <v>4</v>
       </c>
@@ -6756,7 +6768,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>8</v>
       </c>
@@ -6796,7 +6808,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B45">
         <v>8</v>
       </c>
@@ -6810,7 +6822,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B46">
         <v>3</v>
       </c>
@@ -6824,7 +6836,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B47">
         <v>7</v>
       </c>
@@ -6832,7 +6844,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B48">
         <v>6</v>
       </c>
@@ -6840,7 +6852,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>9</v>
       </c>
@@ -6880,7 +6892,7 @@
         <v>178.33333333333331</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B51">
         <v>5</v>
       </c>
@@ -6894,7 +6906,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B52">
         <v>3</v>
       </c>
@@ -6908,7 +6920,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B53">
         <v>2</v>
       </c>
@@ -6916,7 +6928,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B54">
         <v>12</v>
       </c>
@@ -6924,58 +6936,96 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>10</v>
       </c>
       <c r="B56">
         <v>11</v>
       </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="C56">
+        <v>9</v>
+      </c>
+      <c r="D56" t="s">
+        <v>98</v>
+      </c>
+      <c r="E56">
+        <v>3829</v>
+      </c>
+      <c r="F56">
+        <f>E56*100/60-100</f>
+        <v>6281.666666666667</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B57">
         <v>7</v>
       </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="C57">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B58">
         <v>3</v>
       </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="C58">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B59">
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B60">
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>11</v>
       </c>
       <c r="B62">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="C62">
+        <v>9</v>
+      </c>
+      <c r="D62" t="s">
+        <v>98</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <f>E62*100/60-100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B63">
         <v>4</v>
       </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="C63">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B64">
         <v>9</v>
       </c>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="C64">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B65">
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B66">
         <v>5</v>
       </c>

</xml_diff>